<commit_message>
Eksperimenti za časovno zahtevnost
</commit_message>
<xml_diff>
--- a/excel_casovna_p1.xlsx
+++ b/excel_casovna_p1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Spin\PavsicD16$\_System\Desktop\wiener-inverse-interval-problem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darjan - uporabnik\Documents\WIENER-FP\wiener-inverse-interval-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3921D6-D146-4E28-95E7-9571561C2986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="570" yWindow="600" windowWidth="21855" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Velikost grafa (n)</t>
   </si>
@@ -49,11 +50,20 @@
   <si>
     <t>št. dreves za odstranitev</t>
   </si>
+  <si>
+    <t>kmax</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,11 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -106,7 +117,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="sl-SI"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -118,7 +129,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sl-SI"/>
+              <a:t>Časovna zahtevnost P1 v odvisnosti od n</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -565,7 +601,555 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="sl-SI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sl-SI"/>
+              <a:t>Časovna</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sl-SI" baseline="0"/>
+              <a:t> zahtevnost v P1 v odvisnosti od kmax</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sl-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.692825896762905E-2"/>
+          <c:y val="0.12058419243986254"/>
+          <c:w val="0.83329396325459315"/>
+          <c:h val="0.79282382227994697"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Čas (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$33:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>750</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$33:$C$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>1.845</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8580000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1110000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000">
+                  <c:v>2.2240000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.524</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000">
+                  <c:v>2.8079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.000">
+                  <c:v>3.4140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7120000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.3730000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.4349999999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.032</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.000">
+                  <c:v>5.5279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.7069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.2230000000000008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.409000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.042</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.312999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30.414000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37.070999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCBC-4FE3-8A20-83ECB0328543}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="593745184"/>
+        <c:axId val="593745512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="593745184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593745512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="593745512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593745184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sl-SI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1121,24 +1705,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1148,6 +2254,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafikon 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BDB302-0D6F-4EBA-86BE-FECB029D110A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1418,11 +2560,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +2724,7 @@
         <v>30.648</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>350</v>
       </c>
@@ -1590,7 +2732,7 @@
         <v>41.899000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>400</v>
       </c>
@@ -1598,7 +2740,7 @@
         <v>56.039000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>450</v>
       </c>
@@ -1606,7 +2748,7 @@
         <v>70.141000000000005</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>500</v>
       </c>
@@ -1614,7 +2756,7 @@
         <v>87.582999999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>600</v>
       </c>
@@ -1622,7 +2764,7 @@
         <v>128.38999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>700</v>
       </c>
@@ -1630,7 +2772,7 @@
         <v>174.52</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>800</v>
       </c>
@@ -1638,7 +2780,7 @@
         <v>287.35000000000002</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>900</v>
       </c>
@@ -1646,7 +2788,7 @@
         <v>377.34</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1000</v>
       </c>
@@ -1654,7 +2796,7 @@
         <v>481.63</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2000</v>
       </c>
@@ -1662,9 +2804,244 @@
         <v>2686.8</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>3000</v>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1.845</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>1.8580000000000001</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>2.0249999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>2.1110000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>2.1520000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.2240000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>2.4089999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>9</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>2.524</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2.8079999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>25</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3.4140000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46">
+        <v>3.7120000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>4.3730000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48">
+        <v>4.4349999999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>5.032</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>60</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5.5279999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>75</v>
+      </c>
+      <c r="C51">
+        <v>6.7069999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>100</v>
+      </c>
+      <c r="C52">
+        <v>8.2230000000000008</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>150</v>
+      </c>
+      <c r="C53">
+        <v>11.409000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>200</v>
+      </c>
+      <c r="C54">
+        <v>15.042</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>300</v>
+      </c>
+      <c r="C55">
+        <v>22.312999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>400</v>
+      </c>
+      <c r="C56">
+        <v>30.414000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>500</v>
+      </c>
+      <c r="C57">
+        <v>37.070999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>750</v>
+      </c>
+      <c r="C58">
+        <v>52.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novi grafi, končno poročilo
</commit_message>
<xml_diff>
--- a/excel_casovna_p1.xlsx
+++ b/excel_casovna_p1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darjan - uporabnik\Documents\WIENER-FP\wiener-inverse-interval-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50ACFCC-9EFD-444B-AA72-A80E17757940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBC0504-C3CF-4C69-9535-7BBEF05DF780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="0" windowWidth="19635" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2563,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>